<commit_message>
them tim kiem xoa sach
</commit_message>
<xml_diff>
--- a/1712878/FILE/DocGia.xlsx
+++ b/1712878/FILE/DocGia.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nguyen Tho Tuan\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Code\GitHub\OOP_LT_LIRBRARY\1712878\FILE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDCB0F81-BD3D-4E15-863E-791BA347E9A3}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA45B8AE-BFB5-4BF9-8E6B-60E60517CDBE}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="9270" windowHeight="1905" xr2:uid="{F1814635-3D2E-49A6-A180-AF2780D82176}"/>
   </bookViews>
@@ -185,7 +185,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0000000000"/>
+    <numFmt numFmtId="164" formatCode="0000000000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -218,7 +218,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -536,7 +536,7 @@
   <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J28" sqref="J28"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -546,6 +546,7 @@
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -567,75 +568,75 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>278347732</v>
+        <v>210366942</v>
       </c>
       <c r="B2" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="C2" s="1">
-        <v>931396639</v>
+        <v>462854365</v>
       </c>
       <c r="D2" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="E2" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>292185327</v>
+        <v>274299112</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C3" s="1">
-        <v>797620758</v>
+        <v>312982000</v>
       </c>
       <c r="D3" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="E3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>205651265</v>
+        <v>245403375</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C4" s="1">
-        <v>312982000</v>
+        <v>461934945</v>
       </c>
       <c r="D4" t="s">
         <v>35</v>
       </c>
       <c r="E4" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>203617550</v>
+        <v>251262102</v>
       </c>
       <c r="B5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C5" s="1">
-        <v>924000031</v>
+        <v>732841923</v>
       </c>
       <c r="D5" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="E5" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>296731604</v>
+        <v>214587489</v>
       </c>
       <c r="B6" t="s">
         <v>6</v>
@@ -652,24 +653,24 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>255674504</v>
+        <v>268616154</v>
       </c>
       <c r="B7" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C7" s="1">
-        <v>816762743</v>
+        <v>901424984</v>
       </c>
       <c r="D7" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="E7" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>223023947</v>
+        <v>190986546</v>
       </c>
       <c r="B8" t="s">
         <v>9</v>
@@ -686,135 +687,135 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>205447633</v>
+        <v>259937103</v>
       </c>
       <c r="B9" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="C9" s="1">
-        <v>559794230</v>
+        <v>883423258</v>
       </c>
       <c r="D9" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E9" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>281092458</v>
+        <v>226793287</v>
       </c>
       <c r="B10" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="C10" s="1">
-        <v>512555514</v>
+        <v>596234115</v>
       </c>
       <c r="D10" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E10" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>180384048</v>
+        <v>228568444</v>
       </c>
       <c r="B11" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="C11" s="1">
-        <v>901424984</v>
+        <v>749191391</v>
       </c>
       <c r="D11" t="s">
         <v>48</v>
       </c>
       <c r="E11" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>159787679</v>
+        <v>284953322</v>
       </c>
       <c r="B12" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C12" s="1">
-        <v>641379146</v>
+        <v>905842820</v>
       </c>
       <c r="D12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E12" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>150960598</v>
+        <v>223929938</v>
       </c>
       <c r="B13" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="C13" s="1">
-        <v>749191391</v>
+        <v>924000031</v>
       </c>
       <c r="D13" t="s">
         <v>48</v>
       </c>
       <c r="E13" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>154969847</v>
+        <v>216920917</v>
       </c>
       <c r="B14" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C14" s="1">
-        <v>967050075</v>
+        <v>438718377</v>
       </c>
       <c r="D14" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="E14" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>250847870</v>
+        <v>287918095</v>
       </c>
       <c r="B15" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="C15" s="1">
-        <v>579626275</v>
+        <v>512555514</v>
       </c>
       <c r="D15" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="E15" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>235082114</v>
+        <v>165024578</v>
       </c>
       <c r="B16" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="C16" s="1">
-        <v>710123942</v>
+        <v>574040645</v>
       </c>
       <c r="D16" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E16" t="s">
         <v>44</v>
@@ -822,118 +823,118 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>219141175</v>
+        <v>275771181</v>
       </c>
       <c r="B17" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C17" s="1">
-        <v>905842820</v>
+        <v>641379146</v>
       </c>
       <c r="D17" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E17" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>153578779</v>
+        <v>156907345</v>
       </c>
       <c r="B18" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="C18" s="1">
-        <v>883423258</v>
+        <v>816762743</v>
       </c>
       <c r="D18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E18" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>262946414</v>
+        <v>226851874</v>
       </c>
       <c r="B19" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="C19" s="1">
-        <v>574040645</v>
+        <v>385950193</v>
       </c>
       <c r="D19" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E19" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>191029062</v>
+        <v>285206094</v>
       </c>
       <c r="B20" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C20" s="1">
-        <v>993768309</v>
+        <v>311602445</v>
       </c>
       <c r="D20" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="E20" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>205755788</v>
+        <v>166952111</v>
       </c>
       <c r="B21" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C21" s="1">
-        <v>311602445</v>
+        <v>710123942</v>
       </c>
       <c r="D21" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="E21" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>157427389</v>
+        <v>234517495</v>
       </c>
       <c r="B22" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="C22" s="1">
-        <v>438718377</v>
+        <v>931396639</v>
       </c>
       <c r="D22" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E22" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>221488346</v>
+        <v>207232731</v>
       </c>
       <c r="B23" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="C23" s="1">
-        <v>353967350</v>
+        <v>797620758</v>
       </c>
       <c r="D23" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="E23" t="s">
         <v>37</v>
@@ -941,16 +942,16 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>282976970</v>
+        <v>190852217</v>
       </c>
       <c r="B24" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="C24" s="1">
-        <v>596234115</v>
+        <v>503885617</v>
       </c>
       <c r="D24" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E24" t="s">
         <v>40</v>
@@ -958,58 +959,58 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>158306285</v>
+        <v>202321979</v>
       </c>
       <c r="B25" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C25" s="1">
-        <v>732841923</v>
+        <v>993768309</v>
       </c>
       <c r="D25" t="s">
         <v>35</v>
       </c>
       <c r="E25" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>177821368</v>
+        <v>212029163</v>
       </c>
       <c r="B26" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C26" s="1">
-        <v>503885617</v>
+        <v>353967350</v>
       </c>
       <c r="D26" t="s">
         <v>35</v>
       </c>
       <c r="E26" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>205512072</v>
+        <v>270869768</v>
       </c>
       <c r="B27" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="C27" s="1">
-        <v>385950193</v>
+        <v>626876492</v>
       </c>
       <c r="D27" t="s">
         <v>35</v>
       </c>
       <c r="E27" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>279172357</v>
+        <v>232958486</v>
       </c>
       <c r="B28" t="s">
         <v>8</v>
@@ -1026,58 +1027,58 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>220420963</v>
+        <v>179039878</v>
       </c>
       <c r="B29" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C29" s="1">
-        <v>462854365</v>
+        <v>967050075</v>
       </c>
       <c r="D29" t="s">
         <v>48</v>
       </c>
       <c r="E29" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>182421183</v>
+        <v>260493543</v>
       </c>
       <c r="B30" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C30" s="1">
-        <v>626876492</v>
+        <v>579626275</v>
       </c>
       <c r="D30" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="E30" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>264562429</v>
+        <v>188185163</v>
       </c>
       <c r="B31" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="C31" s="1">
-        <v>461934945</v>
+        <v>559794230</v>
       </c>
       <c r="D31" t="s">
         <v>35</v>
       </c>
       <c r="E31" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B1:B35">
-    <sortCondition ref="B1"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E31">
+    <sortCondition ref="A2"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>